<commit_message>
Chen_2002: Updated USDA soil type
</commit_message>
<xml_diff>
--- a/ISRaD_data_files/Chen_2002.xlsx
+++ b/ISRaD_data_files/Chen_2002.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20384"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfromm\Documents\GitHub\ISRaD\ISRaD_data_files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A59B8E8-4C97-42BA-9FB2-B6E03D2CC04D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28440" windowHeight="15020" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28440" windowHeight="15024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="979">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="993">
   <si>
     <t>entry_name</t>
   </si>
@@ -2966,12 +2972,54 @@
   </si>
   <si>
     <t>frc_fraction_modern_sd</t>
+  </si>
+  <si>
+    <t>Ferrasols</t>
+  </si>
+  <si>
+    <t>pro_usda_soil_order</t>
+  </si>
+  <si>
+    <t>Alfisols</t>
+  </si>
+  <si>
+    <t>Andisols</t>
+  </si>
+  <si>
+    <t>Aridisols</t>
+  </si>
+  <si>
+    <t>Entisols</t>
+  </si>
+  <si>
+    <t>Gelisols</t>
+  </si>
+  <si>
+    <t>Histosols</t>
+  </si>
+  <si>
+    <t>Inceptisols</t>
+  </si>
+  <si>
+    <t>Mollisols</t>
+  </si>
+  <si>
+    <t>Oxisols</t>
+  </si>
+  <si>
+    <t>Spodosols</t>
+  </si>
+  <si>
+    <t>Ultisols</t>
+  </si>
+  <si>
+    <t>Vertisols</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3090,10 +3138,18 @@
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_layer" xfId="3"/>
+    <cellStyle name="Normal_layer" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3375,14 +3431,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3432,7 +3490,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3479,7 +3537,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -3517,7 +3575,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -3570,19 +3628,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="25.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3605,7 +3663,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3628,7 +3686,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -3645,7 +3703,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -3662,7 +3720,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -3691,16 +3749,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AK6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3741,76 +3799,79 @@
         <v>84</v>
       </c>
       <c r="N1" t="s">
+        <v>980</v>
+      </c>
+      <c r="O1" t="s">
         <v>85</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>86</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>87</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>88</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>89</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>90</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>91</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>92</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>93</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>94</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>95</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>96</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>97</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>98</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>99</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>100</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>101</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>102</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>103</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>104</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>105</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>106</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3850,77 +3911,77 @@
       <c r="M2" t="s">
         <v>116</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>117</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>118</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>119</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>120</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>121</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>122</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>123</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>124</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>125</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>126</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>127</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>128</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>129</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>130</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>131</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>132</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>133</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>134</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>135</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>136</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>137</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>138</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -3948,29 +4009,26 @@
       <c r="M3" t="s">
         <v>36</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>145</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>146</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>147</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>144</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>148</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>149</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>150</v>
-      </c>
-      <c r="V3" t="s">
-        <v>151</v>
       </c>
       <c r="W3" t="s">
         <v>151</v>
@@ -3979,43 +4037,46 @@
         <v>151</v>
       </c>
       <c r="Y3" t="s">
+        <v>151</v>
+      </c>
+      <c r="Z3" t="s">
         <v>152</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>153</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>154</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>155</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>156</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>157</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>148</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AG3" t="s">
         <v>158</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AH3" t="s">
         <v>159</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>160</v>
       </c>
       <c r="AI3" t="s">
         <v>160</v>
       </c>
       <c r="AJ3" t="s">
+        <v>160</v>
+      </c>
+      <c r="AK3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -4028,14 +4089,23 @@
       <c r="H4" t="s">
         <v>162</v>
       </c>
-      <c r="T4" t="s">
+      <c r="N4" t="s">
+        <v>989</v>
+      </c>
+      <c r="O4" t="s">
+        <v>979</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>823</v>
+      </c>
+      <c r="U4" t="s">
         <v>164</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -4048,14 +4118,23 @@
       <c r="H5" t="s">
         <v>162</v>
       </c>
-      <c r="T5" t="s">
+      <c r="N5" t="s">
+        <v>989</v>
+      </c>
+      <c r="O5" t="s">
+        <v>979</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>823</v>
+      </c>
+      <c r="U5" t="s">
         <v>167</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -4068,10 +4147,19 @@
       <c r="H6" t="s">
         <v>162</v>
       </c>
-      <c r="T6" t="s">
+      <c r="N6" t="s">
+        <v>989</v>
+      </c>
+      <c r="O6" t="s">
+        <v>979</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>823</v>
+      </c>
+      <c r="U6" t="s">
         <v>167</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>168</v>
       </c>
     </row>
@@ -4087,14 +4175,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AK3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4207,7 +4295,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -4317,7 +4405,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -4409,19 +4497,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:CT31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P28" sqref="P28:P31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98">
+    <row r="1" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4717,7 +4805,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="2" spans="1:98">
+    <row r="2" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -5013,7 +5101,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="3" spans="1:98">
+    <row r="3" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -5252,7 +5340,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="4" spans="1:98">
+    <row r="4" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -5287,7 +5375,7 @@
         <v>1.085</v>
       </c>
     </row>
-    <row r="5" spans="1:98">
+    <row r="5" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -5322,7 +5410,7 @@
         <v>1.147</v>
       </c>
     </row>
-    <row r="6" spans="1:98">
+    <row r="6" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -5357,7 +5445,7 @@
         <v>1.1359999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:98">
+    <row r="7" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -5392,7 +5480,7 @@
         <v>1.0659999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:98">
+    <row r="8" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -5427,7 +5515,7 @@
         <v>1.0620000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:98">
+    <row r="9" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -5462,7 +5550,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:98">
+    <row r="10" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -5497,7 +5585,7 @@
         <v>1.0129999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:98">
+    <row r="11" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -5532,7 +5620,7 @@
         <v>0.92900000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:98">
+    <row r="12" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -5567,7 +5655,7 @@
         <v>1.0029999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:98">
+    <row r="13" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -5602,7 +5690,7 @@
         <v>0.89900000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:98">
+    <row r="14" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -5637,7 +5725,7 @@
         <v>0.94099999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:98">
+    <row r="15" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -5672,7 +5760,7 @@
         <v>0.873</v>
       </c>
     </row>
-    <row r="16" spans="1:98">
+    <row r="16" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -5707,7 +5795,7 @@
         <v>0.43200000000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:55">
+    <row r="17" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -5736,7 +5824,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="18" spans="1:55">
+    <row r="18" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -5765,7 +5853,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="19" spans="1:55">
+    <row r="19" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -5794,7 +5882,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="20" spans="1:55">
+    <row r="20" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -5823,7 +5911,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="21" spans="1:55">
+    <row r="21" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -5858,7 +5946,7 @@
         <v>1.242</v>
       </c>
     </row>
-    <row r="22" spans="1:55">
+    <row r="22" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -5893,7 +5981,7 @@
         <v>1.204</v>
       </c>
     </row>
-    <row r="23" spans="1:55">
+    <row r="23" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -5928,7 +6016,7 @@
         <v>1.101</v>
       </c>
     </row>
-    <row r="24" spans="1:55">
+    <row r="24" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -5963,7 +6051,7 @@
         <v>1.0129999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:55">
+    <row r="25" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -5998,7 +6086,7 @@
         <v>0.93099999999999994</v>
       </c>
     </row>
-    <row r="26" spans="1:55">
+    <row r="26" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -6033,7 +6121,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="27" spans="1:55">
+    <row r="27" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -6068,7 +6156,7 @@
         <v>0.80900000000000005</v>
       </c>
     </row>
-    <row r="28" spans="1:55">
+    <row r="28" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -6103,7 +6191,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="29" spans="1:55">
+    <row r="29" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -6138,7 +6226,7 @@
         <v>0.83400000000000007</v>
       </c>
     </row>
-    <row r="30" spans="1:55">
+    <row r="30" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -6173,7 +6261,7 @@
         <v>0.97099999999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:55">
+    <row r="31" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -6224,14 +6312,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6317,7 +6405,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -6400,7 +6488,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -6459,16 +6547,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BU3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+    <sheetView topLeftCell="AG1" workbookViewId="0">
       <selection activeCell="AI1" sqref="AI1:AK1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:73" ht="52">
+    <row r="1" spans="1:73" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6689,7 +6777,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="2" spans="1:73">
+    <row r="2" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -6907,7 +6995,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="3" spans="1:73">
+    <row r="3" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -7086,14 +7174,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AD3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7185,7 +7273,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -7268,7 +7356,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -7327,14 +7415,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:AS21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:44">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>736</v>
       </c>
@@ -7347,128 +7437,128 @@
       <c r="D1" t="s">
         <v>739</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>740</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>741</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>742</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>743</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>744</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>745</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>746</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>747</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>748</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>749</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>750</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>751</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>752</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>753</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>754</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>755</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>756</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>757</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>758</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>759</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>760</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>761</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>762</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>763</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>764</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>765</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>766</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>767</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>768</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>769</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>770</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>771</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>772</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>773</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>774</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>775</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>776</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>777</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>778</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>779</v>
       </c>
     </row>
-    <row r="2" spans="1:44">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -7482,150 +7572,153 @@
         <v>103</v>
       </c>
       <c r="E2" t="s">
+        <v>980</v>
+      </c>
+      <c r="F2" t="s">
         <v>87</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>91</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>104</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>96</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>97</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>99</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>79</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>175</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>177</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>178</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>179</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>181</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>183</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>184</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>185</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>191</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>268</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>273</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>302</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>252</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>256</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>259</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>780</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>552</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>553</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>554</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>555</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>561</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>691</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>781</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>697</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>699</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>701</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>704</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AN2" t="s">
         <v>594</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>598</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>593</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>595</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
         <v>600</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="3" spans="1:44">
-      <c r="G3" t="s">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
         <v>782</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>783</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>784</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>783</v>
       </c>
-      <c r="AM3" t="s">
+      <c r="AN3" t="s">
         <v>660</v>
       </c>
-      <c r="AO3" t="s">
+      <c r="AP3" t="s">
         <v>785</v>
       </c>
-      <c r="AP3" t="s">
+      <c r="AQ3" t="s">
         <v>786</v>
       </c>
     </row>
-    <row r="4" spans="1:44">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>787</v>
       </c>
@@ -7639,127 +7732,130 @@
         <v>790</v>
       </c>
       <c r="E4" t="s">
+        <v>981</v>
+      </c>
+      <c r="F4" t="s">
         <v>163</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>791</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>792</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>793</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>794</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>795</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>162</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>796</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>797</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>798</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>799</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>800</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>801</v>
-      </c>
-      <c r="R4" t="s">
-        <v>789</v>
       </c>
       <c r="S4" t="s">
         <v>789</v>
       </c>
       <c r="T4" t="s">
+        <v>789</v>
+      </c>
+      <c r="U4" t="s">
         <v>802</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>803</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>804</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>805</v>
-      </c>
-      <c r="X4" t="s">
-        <v>789</v>
       </c>
       <c r="Y4" t="s">
         <v>789</v>
       </c>
       <c r="Z4" t="s">
+        <v>789</v>
+      </c>
+      <c r="AA4" t="s">
         <v>806</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>807</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>808</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>797</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>809</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AF4" t="s">
         <v>800</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AG4" t="s">
         <v>810</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AH4" t="s">
         <v>811</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" t="s">
         <v>798</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AJ4" t="s">
         <v>812</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AK4" t="s">
         <v>813</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AL4" t="s">
         <v>814</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="AM4" t="s">
         <v>815</v>
       </c>
-      <c r="AM4" t="s">
+      <c r="AN4" t="s">
         <v>816</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AO4" t="s">
         <v>817</v>
       </c>
-      <c r="AO4" t="s">
+      <c r="AP4" t="s">
         <v>818</v>
       </c>
-      <c r="AP4" t="s">
+      <c r="AQ4" t="s">
         <v>819</v>
       </c>
-      <c r="AQ4" t="s">
+      <c r="AR4" t="s">
         <v>789</v>
       </c>
-      <c r="AR4" t="s">
+      <c r="AS4" t="s">
         <v>805</v>
       </c>
     </row>
-    <row r="5" spans="1:44">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>820</v>
       </c>
@@ -7770,109 +7866,112 @@
         <v>822</v>
       </c>
       <c r="E5" t="s">
+        <v>982</v>
+      </c>
+      <c r="F5" t="s">
         <v>823</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>824</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>825</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>826</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>827</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>828</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>829</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>830</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>831</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>832</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>833</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>834</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>835</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>836</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>837</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>838</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>839</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>840</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>841</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>831</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>842</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>834</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AG5" t="s">
         <v>843</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AH5" t="s">
         <v>844</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AI5" t="s">
         <v>832</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AJ5" t="s">
         <v>845</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AK5" t="s">
         <v>846</v>
       </c>
-      <c r="AK5" t="s">
+      <c r="AL5" t="s">
         <v>847</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="AM5" t="s">
         <v>848</v>
       </c>
-      <c r="AM5" t="s">
+      <c r="AN5" t="s">
         <v>849</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AO5" t="s">
         <v>850</v>
       </c>
-      <c r="AO5" t="s">
+      <c r="AP5" t="s">
         <v>851</v>
       </c>
-      <c r="AP5" t="s">
+      <c r="AQ5" t="s">
         <v>852</v>
       </c>
-      <c r="AR5" t="s">
+      <c r="AS5" t="s">
         <v>839</v>
       </c>
     </row>
-    <row r="6" spans="1:44">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>853</v>
       </c>
@@ -7883,447 +7982,477 @@
         <v>855</v>
       </c>
       <c r="E6" t="s">
+        <v>983</v>
+      </c>
+      <c r="F6" t="s">
         <v>856</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>167</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>857</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>858</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>859</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>860</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>861</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>862</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>863</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>864</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>865</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>590</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>866</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>867</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>868</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>869</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>870</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>871</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>862</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>865</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AG6" t="s">
         <v>872</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AH6" t="s">
         <v>873</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AI6" t="s">
         <v>874</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AJ6" t="s">
         <v>875</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AK6" t="s">
         <v>856</v>
       </c>
-      <c r="AM6" t="s">
+      <c r="AN6" t="s">
         <v>876</v>
       </c>
-      <c r="AN6" t="s">
+      <c r="AO6" t="s">
         <v>877</v>
       </c>
-      <c r="AO6" t="s">
+      <c r="AP6" t="s">
         <v>878</v>
       </c>
-      <c r="AP6" t="s">
+      <c r="AQ6" t="s">
         <v>36</v>
       </c>
-      <c r="AR6" t="s">
+      <c r="AS6" t="s">
         <v>869</v>
       </c>
     </row>
-    <row r="7" spans="1:44">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>879</v>
       </c>
       <c r="B7" t="s">
         <v>880</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E7" t="s">
+        <v>984</v>
+      </c>
+      <c r="G7" t="s">
         <v>881</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>882</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>883</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>884</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>885</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>886</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>887</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>888</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>889</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>890</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>891</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>892</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>886</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AF7" t="s">
         <v>888</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AG7" t="s">
         <v>893</v>
       </c>
-      <c r="AG7" t="s">
+      <c r="AH7" t="s">
         <v>894</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AJ7" t="s">
         <v>895</v>
       </c>
-      <c r="AM7" t="s">
+      <c r="AN7" t="s">
         <v>896</v>
       </c>
-      <c r="AN7" t="s">
+      <c r="AO7" t="s">
         <v>897</v>
       </c>
-      <c r="AO7" t="s">
+      <c r="AP7" t="s">
         <v>898</v>
       </c>
-      <c r="AP7" t="s">
+      <c r="AQ7" t="s">
         <v>899</v>
       </c>
-      <c r="AR7" t="s">
+      <c r="AS7" t="s">
         <v>892</v>
       </c>
     </row>
-    <row r="8" spans="1:44">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>900</v>
       </c>
       <c r="B8" t="s">
         <v>901</v>
       </c>
-      <c r="F8" t="s">
+      <c r="E8" t="s">
+        <v>985</v>
+      </c>
+      <c r="G8" t="s">
         <v>164</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>902</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>903</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>904</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>905</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>906</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>907</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>908</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>909</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>910</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>911</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>856</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AD8" t="s">
         <v>906</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AF8" t="s">
         <v>908</v>
       </c>
-      <c r="AG8" t="s">
+      <c r="AH8" t="s">
         <v>912</v>
       </c>
-      <c r="AM8" t="s">
+      <c r="AN8" t="s">
         <v>913</v>
       </c>
-      <c r="AN8" t="s">
+      <c r="AO8" t="s">
         <v>914</v>
       </c>
-      <c r="AO8" t="s">
+      <c r="AP8" t="s">
         <v>915</v>
       </c>
-      <c r="AP8" t="s">
+      <c r="AQ8" t="s">
         <v>590</v>
       </c>
-      <c r="AR8" t="s">
+      <c r="AS8" t="s">
         <v>856</v>
       </c>
     </row>
-    <row r="9" spans="1:44">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>916</v>
       </c>
       <c r="B9" t="s">
         <v>917</v>
       </c>
-      <c r="F9" t="s">
+      <c r="E9" t="s">
+        <v>986</v>
+      </c>
+      <c r="G9" t="s">
         <v>918</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>919</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>920</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>921</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>922</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>923</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>924</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>925</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>926</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AF9" t="s">
         <v>927</v>
       </c>
-      <c r="AG9" t="s">
+      <c r="AH9" t="s">
         <v>923</v>
       </c>
-      <c r="AM9" t="s">
+      <c r="AN9" t="s">
         <v>928</v>
       </c>
-      <c r="AN9" t="s">
+      <c r="AO9" t="s">
         <v>929</v>
       </c>
-      <c r="AO9" t="s">
+      <c r="AP9" t="s">
         <v>930</v>
       </c>
-      <c r="AP9" t="s">
+      <c r="AQ9" t="s">
         <v>931</v>
       </c>
     </row>
-    <row r="10" spans="1:44">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>932</v>
       </c>
       <c r="B10" t="s">
         <v>933</v>
       </c>
-      <c r="F10" t="s">
+      <c r="E10" t="s">
+        <v>987</v>
+      </c>
+      <c r="G10" t="s">
         <v>934</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>935</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>936</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="s">
         <v>937</v>
       </c>
-      <c r="AM10" t="s">
+      <c r="AN10" t="s">
         <v>938</v>
       </c>
-      <c r="AN10" t="s">
+      <c r="AO10" t="s">
         <v>939</v>
       </c>
-      <c r="AO10" t="s">
+      <c r="AP10" t="s">
         <v>940</v>
       </c>
-      <c r="AP10" t="s">
+      <c r="AQ10" t="s">
         <v>941</v>
       </c>
     </row>
-    <row r="11" spans="1:44">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>942</v>
       </c>
-      <c r="F11" t="s">
+      <c r="E11" t="s">
+        <v>988</v>
+      </c>
+      <c r="G11" t="s">
         <v>943</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>944</v>
       </c>
-      <c r="U11" t="s">
+      <c r="V11" t="s">
         <v>945</v>
       </c>
-      <c r="AM11" t="s">
+      <c r="AN11" t="s">
         <v>946</v>
-      </c>
-      <c r="AN11" t="s">
-        <v>947</v>
       </c>
       <c r="AO11" t="s">
         <v>947</v>
       </c>
       <c r="AP11" t="s">
+        <v>947</v>
+      </c>
+      <c r="AQ11" t="s">
         <v>948</v>
       </c>
     </row>
-    <row r="12" spans="1:44">
-      <c r="H12" t="s">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>989</v>
+      </c>
+      <c r="I12" t="s">
         <v>949</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" t="s">
         <v>950</v>
       </c>
-      <c r="AM12" t="s">
+      <c r="AN12" t="s">
         <v>951</v>
       </c>
-      <c r="AN12" t="s">
+      <c r="AO12" t="s">
         <v>952</v>
       </c>
-      <c r="AO12" t="s">
+      <c r="AP12" t="s">
         <v>953</v>
       </c>
     </row>
-    <row r="13" spans="1:44">
-      <c r="U13" t="s">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>990</v>
+      </c>
+      <c r="V13" t="s">
         <v>954</v>
       </c>
-      <c r="AM13" t="s">
+      <c r="AN13" t="s">
         <v>955</v>
       </c>
-      <c r="AN13" t="s">
+      <c r="AO13" t="s">
         <v>956</v>
       </c>
-      <c r="AO13" t="s">
+      <c r="AP13" t="s">
         <v>957</v>
       </c>
     </row>
-    <row r="14" spans="1:44">
-      <c r="U14" t="s">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>991</v>
+      </c>
+      <c r="V14" t="s">
         <v>958</v>
       </c>
-      <c r="AN14" t="s">
+      <c r="AO14" t="s">
         <v>959</v>
       </c>
-      <c r="AO14" t="s">
+      <c r="AP14" t="s">
         <v>960</v>
       </c>
     </row>
-    <row r="15" spans="1:44">
-      <c r="U15" t="s">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>992</v>
+      </c>
+      <c r="V15" t="s">
         <v>961</v>
       </c>
-      <c r="AN15" t="s">
+      <c r="AO15" t="s">
         <v>962</v>
       </c>
-      <c r="AO15" t="s">
+      <c r="AP15" t="s">
         <v>963</v>
       </c>
     </row>
-    <row r="16" spans="1:44">
-      <c r="U16" t="s">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="V16" t="s">
         <v>964</v>
       </c>
-      <c r="AN16" t="s">
+      <c r="AO16" t="s">
         <v>965</v>
       </c>
-      <c r="AO16" t="s">
+      <c r="AP16" t="s">
         <v>966</v>
       </c>
     </row>
-    <row r="17" spans="40:41">
-      <c r="AN17" t="s">
+    <row r="17" spans="41:42" x14ac:dyDescent="0.3">
+      <c r="AO17" t="s">
         <v>967</v>
       </c>
-      <c r="AO17" t="s">
+      <c r="AP17" t="s">
         <v>968</v>
       </c>
     </row>
-    <row r="18" spans="40:41">
-      <c r="AN18" t="s">
+    <row r="18" spans="41:42" x14ac:dyDescent="0.3">
+      <c r="AO18" t="s">
         <v>969</v>
       </c>
-      <c r="AO18" t="s">
+      <c r="AP18" t="s">
         <v>970</v>
       </c>
     </row>
-    <row r="19" spans="40:41">
-      <c r="AN19" t="s">
+    <row r="19" spans="41:42" x14ac:dyDescent="0.3">
+      <c r="AO19" t="s">
         <v>971</v>
       </c>
-      <c r="AO19" t="s">
+      <c r="AP19" t="s">
         <v>972</v>
       </c>
     </row>
-    <row r="20" spans="40:41">
-      <c r="AN20" t="s">
+    <row r="20" spans="41:42" x14ac:dyDescent="0.3">
+      <c r="AO20" t="s">
         <v>973</v>
       </c>
-      <c r="AO20" t="s">
+      <c r="AP20" t="s">
         <v>974</v>
       </c>
     </row>
-    <row r="21" spans="40:41">
-      <c r="AN21" t="s">
+    <row r="21" spans="41:42" x14ac:dyDescent="0.3">
+      <c r="AO21" t="s">
         <v>975</v>
       </c>
     </row>

</xml_diff>